<commit_message>
research: GPT 4o mini 청크 2000, 2500, 3000, 3500(0~300) 오버랩 조정 실험 결과
</commit_message>
<xml_diff>
--- a/deuChatbot/test_automation/real_qna.xlsx
+++ b/deuChatbot/test_automation/real_qna.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\DeuChatbot\deuChatbot\test_automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E7A641-B767-49EA-B29D-6ACE8B7AEF0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B66C7F9-413A-46B2-8EF4-A3AD77A7D9A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ABFFA3B5-2554-4543-A201-B6E726E2138D}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="232">
   <si>
     <t>질의</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1314,685 +1314,9 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>간호학과 정시 성적이 3.7인데 정시 전형 합격할 수 있을까요…?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>간호학과의 최종등록자 데이터를 기준으로 보면, 간호학과의 영어 등급 평균은 2.34이고, 수능 4개 영역 등급 평균은 3.37입니다. 
 따라서, 현재 정시 등급이 3.7이라면 간호학과의 평균 등급보다 낮은 성적을 가지고 있기 때문에 합격 가능성이 낮습니다. 
 자세한 사항은 "https://ipsi.deu.ac.kr/main.do"에서 확인하시기 바랍니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>디자인조형학과의 실기시험은 "기초디자인 / 사고의 전환" 중에서 하나를 선택하여 응시하게 되며, 실기 점수는 전체 평가의 70%를 차지합니다. 이 실기시험은 정시 나군 실기/실적 일반학생전형에 속하는데, 평가 비율은 수능 30%, 실기 70%로 구성됩니다. 실기시험을 위해서는 수험표와 사진, 생년월일이 포함된 신분증을 지참해야 하며, 실기시험에 불참하거나 한 종목도 불참할 경우 불합격 처리됩니다. 배점은 전형총점 1,000점 만점 기준으로 700점이 할당됩니다 .</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>다시 질문 부탁드립니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>디자인조형학과의 기초디자인 실기시험 주제는 '기초디자인'과 '사고의 전환' 두 가지 주제가 있습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2024학년도 정시 가군 인문사회과학대학 국어국문학과 일반학생 전형으로 10명을 모집합니다 .</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>네, 정시 나군 실기/실기 경기실적우수자 전형인 경기지도학과에서는 출결 점수가 평가에 반영됩니다. 이 전형에서는 학생부교과 18%, 출결 12%, 서류 70%를 평가에 반영한다고 되어 있습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2024학년도 동의대학교 인문사회과학대학 영어영문학과의 다군 일반학생 전형으로는 총 24명을 모집합니다 .</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>2024</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF212529"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>학년도</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF212529"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF212529"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>의료보건생활대학</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF212529"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF212529"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>간호학과</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF212529"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF212529"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>나군</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF212529"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF212529"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>일반학생</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF212529"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF212529"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>전형의</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF212529"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF212529"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>모집</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF212529"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF212529"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>인원은</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF212529"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> 23</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF212529"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>명입니다</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF212529"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> .</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>수능 영어 영역 등급에 따른 점수는 다음과 같습니다:
-- 1등급: 139점
-- 2등급: 131점
-- 3등급: 123점
-- 4등급: 115점
-- 5등급: 107점
-- 6등급: 99점
-- 7등급: 91점
-- 8등급: 83점
-- 9등급: 75점 .</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>예술고 학생이더라도 나군 학생부교과 농어촌학생전형으로 지원하는 데 특별한 제한은 없어 보입니다. 이 전형의 지원 자격은 부모의 거주지와 상관없이 지원자 본인이 초등학교, 중학교, 고등학교 전 과정을 농어촌(읍·면)지역 소재 학교에서 이수하고 거주한 자로 되어 있으며, 해당 요건을 충족하는 지원자라면 예술고 출신 여부와 상관없이 지원 가능합니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>경기지도학과의 전형 요소 반영 비율은 학생부교과 18%, 출결 12%, 서류(경기실적) 70%입니다 .</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2024학년도 정시 가군에서 물리치료학과는 총 5명을 모집합니다 .</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2024학년도 정시 나군 실기/실적 전형에서 디자인조형학과의 실기고사는 2024년 1월 17일 수요일에 진행됩니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>동의대학교 2024학년도 정시 다군 수능 일반학생 전형에는 수능 최저학력기준이 없습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>동의대학교의 2024학년도에 신설된 학과는 다음과 같습니다:
-- 심리치료학과
-- 스마트항만물류학과
-- 창업투자경영학과
-- 라이프융합학부(스타트업창업투자학, 뷰티비지니스학, 라이프생활문화학)
-- 경기지도학과 .</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>본 서비스는 정시 모집 전형에 국한하여 서비스를 제공합니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>동의대학교에서는 의료·보건·생활대학, 공과대학, ICT융합공과대학 모집단위에서 수능 가산점을 적용합니다. 구체적으로, 수학(미적분 또는 기하) 응시자에게는 수학 취득 표준점수의 10%를 가산점으로 부여합니다 .</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2024학년도 동의대학교 정시 가군 실기고사(음악학과, 레저스포츠학과, 태권도학과)는 2024년 1월 16일 화요일에 진행됩니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2024학년도 동의대학교 정시 나군 수능(일반학생전형) 전형에서는 한의예과, 디자인조형학과, 체육학과, 경기지도학과가 제외됩니다. 나머지 모든 모집 단위의 평가 기준은 수능 100%이며, 수능 최저학력기준이 없습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2024학년도 동의대학교 정시 가군에서의 수능 성적 반영 방법은 다음과 같습니다. 국어, 수학, 영어, 탐구 영역 각각을 25%씩 반영합니다. 국어는 화법과 작문 또는 언어와 매체 중 선택하여 반영하고, 수학은 확률과 통계 또는 미적분 또는 기하 중 선택하여 반영합니다. 탐구 영역은 사회탐구, 과학탐구, 직업탐구 중 선택한 두 과목의 표준점수를 합산하여 반영합니다 .
-또한, 수능 영어 영역은 등급에 따른 점수로 반영되며, 1등급은 139점부터 9등급은 75점까지 반영됩니다 . 음악학과, 레저스포츠학과, 태권도학과를 제외한 정시 가군 수능(일반학생전형)의 전 모집단위는 수능 성적을 100% 반영합니다 .
-한국사 영역은 반드시 응시해야 하며, 일부 전형에서는 수학(미적분 또는 기하) 응시자에게 수학 표준점수의 0.1을 가산점으로 부여합니다 . 구체적인 전형에 따른 세부 사항은 동의대학교의 정시 입시요강을 참고하시기 바랍니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>정시 다군 수능 일반학생 전형은 수능 최저학력기준이 없음을 명시하고 있습니다 .</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2024학년도에 동의대학교에서 학부에서 학과로 분리된 학과는 다음과 같습니다:
-1. 화학공학과, 환경공학과, 응용화학과: 이전 학년도에서는 화학환경공학부로 통합되어 있었습니다 .
-2. 의생명공학과, 바이오의약공학과, 식품공학과: 이전 학년도에서는 바이오응용공학부로 통합되어 있었습니다 .
-3. 인간공학과, 제품디자인공학과: 이전 학년도에서는 통합된 학부 명칭이 제공되지 않았지만 분리되었다고 명시되어 있습니다 .
-4. 경영정보학과, e비지니스학과: 이전 학년도에서는 정보경영학부로 통합되어 있었습니다 .
-5. 기계공학과, 로봇자동화공학과, 자동차공학과: 이전 학년도에서는 기계자동차로봇부품공학부로 통합되어 있었습니다 .
-6. 신소재공학과, 고분자나노공학과: 이전 학년도에서는 신소재공학부로 통합되어 있었습니다 .
-7. 건축학과(5년제), 건축공학과, 토목공학과, 도시공학과: 이전 학년도에서는 건설공학부로 통합되어 있었습니다 .
-8. 전기공학과, 전자공학과: 이전 학년도에서는 전기전자통신공학부로 통합되어 있었습니다 .
-이러한 분리는 각 학과가 각각 독립적인 모집단위로 운영될 것임을 의미합니다. 추가적인 정보가 필요하시다면, 2024학년도 정시 입시요강 자료를 참고하시거나 입학관리팀으로 문의하시기 바랍니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>동의대학교의 2024학년도 정시 원서접수 마감일은 2024년 1월 6일(토요일) 18시까지입니다 .</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2024학년도에는 정시 나군 실기/실적 경기실적우수자전형에서 변화가 있습니다. 이 전형의 수능 최저학력기준은 없으며, 수능 미응시자도 지원이 가능합니다. 또한, 전형 요소 반영 비율이 학생부교과 18%, 출결 12%, 서류(경기실적) 70%로 설정되어 있습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2024학년도 동의대학교 정시 가군 실기/실적 일반학생 전형에서 실기의 비중은 70%이며, 수능의 비중은 30%입니다 .</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>동의대학교의 라이프융합학부는 2024학년도에 스타트업창업투자학, 뷰티비지니스학, 라이프생활문화학의 세부 전공으로 구성되어 있습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2024학년도 동의대학교 정시 가군에서 실기고사에 참여해야 하는 학과는 음악학과, 레저스포츠학과, 태권도학과입니다. 이들 학과는 실기 점수를 70% 반영하고, 수능 점수를 30% 반영합니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2024학년도 동의대학교 실기/실적 위주 전형으로 지원 가능한 학과는 다음과 같습니다:
-- 가군에 속하는 학과:
-- 음악학과
-- 레저스포츠학과
-- 태권도학과
-이들 학과는 실기 70%, 수능 30%를 반영합니다.
-- 나군에 속하는 학과:
-- 디자인조형학과
-- 체육학과
-이들 학과 또한 실기 70%, 수능 30%를 반영합니다【9†source】.
-- 나군 실기/실적 경기실적우수자 전형은 다음과 같은 반영 비율을 가집니다:
-- 학생부교과 18%
-- 출결 12%
-- 서류 70%【9†source】.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>정시 입시요강 내에서 라이프융합학부에 대한 구체적인 정보나 제공되는 전공에 대한 자료를 찾는 데 어려움이 있습니다. 입학관리팀에게 문의하시거나 동의대학교 입학안내 홈페이지(http://ipsi.deu.ac.kr)에서 라이프융합학부에 관련된 추가 정보를 확인하시는 것을 추천드립니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>네, 특수목적고등학교 학생도 동의대학교 정시 나군 수능 일반학생전형에 지원이 가능합니다. 고교 유형별로 일반고, 자율고, 과학고, 국제고, 외국어고, 예술고, 체육과, 마이스터고, 특성(직업), 특성(대안), 영재학교, 기타 학력인정고, 방송통신고, 각종 학교, 검정고시, 외국고까지 포함하여 모두 지원 가능함을 기재하고 있습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2024학년도 동의대학교 정시 나군 전형에서 가장 많이 모집하는 학과는 ICT융합공과대학의 전기공학과로, 총 35명을 모집합니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>네, 동의대학교의 2024학년도 정시 모집 학생부교과 농어촌학생전형의 12년 과정 지원 자격에 따르면 부모의 거주지와는 상관없이 지원자 본인이 초등학교, 중학교, 고등학교 전 과정을 농어촌(읍·면)지역 소재 학교에서 이수하고 거주한 경우에 지원이 가능합니다. 여기서 중요한 점은 특정 학교 유형(예: 특수목적고등학교)에 대한 언급이 없으므로, 교육 과정을 농어촌 지역 소재 학교에서 이수했을 경우 특수목적고든 일반고든 지원이 가능할 것 같습니다. 그러나 이 부분은 명확한 확인을 위해 입학관리팀에 문의하는 것이 좋을 것 같습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2024학년도 동의대학교 ICT융합공과대학 창의소프트웨어공학부의 합격자 평균 성적은 다음과 같습니다:
-- 수능 4개 영역 표준(변환) 점수합 평균: 450.71
-- 국어+수학+탐구(2개) 표준(변환) 점수 평균: 330.11
-- 영어등급 평균: 3.30
-- 수능 4개 영역등급 평균: 4.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2024학년도 동의대학교 ICT융합공과대학 창의소프트웨어공학부의 최초 합격자들의 평균 성적은 다음과 같습니다:
-- 수능 4개 영역 표준(변환)점수합 평균: 450.71
-- 국어, 수학, 탐구(2개) 표준(변환)점수 평균: 330.11
-- 영어 등급 평균: 3.30
-- 수능 4개 영역 등급 평균: 4.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>동의대학교 2024학년도 정시 최초 합격자 발표는 2024년 2월 2일 금요일 오후 2시에 진행됩니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>정시 나군 면접고사는 2024년 1월 20일(토)에 진행됩니다. 면접고사 대기실 및 입실시간은 2024년 1월 12일(금) 14:00 이후에 입학안내 홈페이지에서 조회할 수 있습니다 .</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2024학년도 동의대학교 정시 나군 수능 일반학생 전형에서 한의예과를 포함한 대부분의 모집 단위는 수능 점수 100%를 반영하여 평가하고, 수능 최저학력기준은 제시하지 않습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>정시 다군 수능 일반학생 전형에서는 수능 최저학력기준이 없습니다 .</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>충원합격자 발표 기간은 2024년 2월 15일(목)부터 2024년 2월 20일(화)까지입니다. 이 기간 동안 전화 연락을 놓치지 않도록 유의해야 합니다 .</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>동의대학교 2024학년도 정시 충원 합격자의 1차 발표는 2024년 2월 14일(수) 오전 9시부터이며, 2차 발표는 2024년 2월 15일(목) 오전 9시에 이뤄집니다. 3차 이후 충원 합격자 발표는 2024년 2월 15일(목) 오후 7시부터 시작하여 2024년 2월 20일(화) 오후 6시까지 이루어질 예정입니다. 3차 이후의 발표는 개별 전화 통보로 진행됩니다 .</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>정시 모집인원은 수시모집 결과에 따라 증가될 수 있으며, 확정된 모집인원은 2024년 1월 2일 화요일에 입학 안내 홈페이지를 통해 공고할 예정입니다. 추가모집에 대한 구체적인 내용은 제공된 문서에서 직접 확인할 수 없으므로 홈페이지에서 공고되는 정보를 확인하시길 권장합니다.
-[입학 안내 홈페이지](http://ipsi.deu.ac.kr)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2024학년도 정시 나군 학생부종합 평생학습자 전형의 평가는 서류 70%, 면접 30%를 반영합니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>동의대학교 2024학년도 정시 나군 학생부종합 평생학습자전형의 평가는 서류 70%, 면접 30%를 반영합니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>실기고사에 대한 구체적인 장소 정보는 제공된 문서에 명시되어 있지 않습니다. 다만, 실기고사 대기실 및 입실시간에 대한 안내는 2024년 1월 12일 금요일 14시 이후에 입학안내 홈페이지에서 확인할 수 있습니다.구체적인 장소를 알고 싶으시다면, 안내된 일정이 되면 입학안내 홈페이지를 통해 확인하시길 바랍니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>체육학과의 실기고사는 2024년 1월 17일 수요일에 진행되며, 실기고사 대기실 및 입실시간 등의 구체적인 안내는 2024년 1월 12일 금요일 14:00 이후에 입학안내 홈페이지에서 조회하실 수 있습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>동의대학교 2024학년도 정시 모집에서 수능 미응시자도 지원 가능한 전형이 있습니다. 정시 나군의 '실기/실적 경기실적우수자전형'은 수능 최저학력기준이 없으며, 수능 미응시자도 지원할 수 있습니다 . 다른 전형에 관한 정보는 정시 입시요강을 확인하거나 입학관리팀에 문의하여야 할 수 있습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>고등학교 졸업한 지 10년이 지난 경우에 대한 구체적인 언급을 찾지 못했습니다. 그러나 제공된 자료에서 정시 가군 수능 일반학생전형의 지원 자격은 "고교 졸업(예정)자 또는 기타 법령에 의하여 이와 동등 이상의 학력이 있다고 인정된 자"로 정의되어 있습니다. 따라서 고등학교 졸업한 지 10년이 지났어도, 동등 이상의 학력을 인정받는 경우 정시 전형에 지원이 가능할 것으로 보입니다. 확실한 정보를 위해서는 2024학년도 정시 입시요강 자료를 참고하거나 입학관리팀에 직접 문의하는 것이 좋겠습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2024학년도 동의대학교 정시 입시 일정은 다음과 같습니다.
-- 정시 모집인원 확정 공고: 2024년 1월 2일(화요일)
-- 원서 접수(인터넷): 2024년 1월 3일(수요일)부터 1월 6일(토요일) 오후 6시까지
-접수 사이트: http://ipsi.deu.ac.kr, http://www.uwayapply.com
-- 서류 제출(제출 서류가 있는 경우): 2024년 1월 3일(수요일)부터 1월 12일(금요일) 오후 5시까지 도착분 유효
-- 정시 가군 실기고사(음악학과, 레저스포츠학과, 태권도학과): 2024년 1월 16일(화요일)
-- 정시 나군 실기고사(디자인조형학과, 체육학과): 2024년 1월 17일(수요일)
-실기고사 대기실 및 입실시간 안내: 2024년 1월 12일(금요일) 오후 2시 이후 입학안내 홈페이지에서 조회
-- 정시 나군 면접고사(다양한 특별전형): 2024년 1월 20일(토요일)
-면접고사 대기실 및 입실시간 안내: 2024년 1월 12일(금요일) 오후 2시 이후 입학안내 홈페이지에서 조회
-- 정시 최초 합격자 발표(가군, 나군, 다군): 2024년 2월 2일(금요일) 오후 2시
-- 정시 최초 합격자 등록(가군, 나군, 다군): 2024년 2월 7일(수요일)부터 2월 13일(화요일)까지
-- 정시 충원 합격자 발표 및 등록: 2024년 2월 14일(수요일) 부터 2월 20일(화요일)까지 여러 차례에 걸쳐 진행
-모든 지원자는 전형 일정에 명시된 합격자 발표일에 홈페이지에서 합격 여부를 확인해야 하며, 등록금 납부 기일을 지켜야 합니다. 만약 합격 여부를 확인하지 않아 등록하지 못한 경우에는 등록(입학) 포기자로 간주됩니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>동의대학교 정시 모집 전형 중 수능 미응시자도 지원 가능한 전형으로는 '정시 나군 실기/실적 경기실적우수자전형'이 있습니다. 이 전형은 수능 최저학력기준이 없으며, 수능 미응시자 역시 지원할 수 있습니다 . 기타 전형에 대해서 확인이 필요하시다면, 2024학년도 정시 입시요강 자료를 참고하시거나 입학관리팀에 문의하시길 권장합니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>전년도 동의대학교 전자공학과의 충원 합격 차수에 관한 정보를 현재 제공된 자료에서 찾을 수 없습니다. 자세한 정보는 2024학년도 정시 입시요강 자료를 참고하거나 입학관리팀에 문의하실 것을 안내드립니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2024학년도 동의대학교 정시 모집 일정은 다음과 같습니다:
-- 정시 모집인원 확정 공고: 2024년 1월 2일(화요일), 입학안내 홈페이지 공고
-- 원서 접수 (인터넷): 2024년 1월 3일(수)부터 1월 6일(토)까지, 마감일 오후 6시까지 ([입시 홈페이지](http://ipsi.deu.ac.kr), [Uwayapply](http://www.uwayapply.com))
-- 서류 제출 (제출 서류가 있는 경우): 2024년 1월 3일(수)부터 1월 12일(금)까지, 마감일 오후 5시까지 도착
-- 정시 가군 실기고사(음악학과, 레저스포츠학과, 태권도학과): 2024년 1월 16일(화)
-- 정시 나군 실기고사(디자인조형학과, 체육학과): 2024년 1월 17일(수)
-- 정시 나군 면접고사(특정 전형): 2024년 1월 20일(토)
-- 정시 최초 합격자 발표 (가군, 나군, 다군): 2024년 2월 2일(금) 오후 2시
-- 정시 최초 합격자 등록 (가군, 나군, 다군): 2024년 2월 7일(수)부터 2월 13일(화)까지 (은행마감시간 내)
-- 정시 충원 합격자 발표 및 등록(1차, 2차, 3차 이후): 2024년 2월 14일(수)부터 2월 20일(화)까지
-정시 최초 합격자 및 충원 합격자 발표는 홈페이지를 통해 확인 가능하며, 등록금 고지서는 홈페이지에서 출력하거나 입학관리팀에서 수령할 수 있습니다. 모든 지원자는 합격 여부를 홈페이지를 통해 확인해야 하며, 확인하지 못해 등록을 하지 않을 경우 입학 포기자로 간주됩니다.
-출처: 동의대학교 정시 입시요강.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>검색 결과 입학처의 전화번호에 대한 직접적인 정보를 찾을 수 없습니다. 입학처 전화번호는 2024학년도 정시 입시요강 자료에 포함되어 있을 가능성이 높으니, 해당 문서를 참고하시거나 동의대학교 입학안내 홈페이지(http://ipsi.deu.ac.kr)을 방문하시거나 입학관리팀에 직접 문의하시는 것을 권장드립니다 .</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3차 이후 충원합격자에 대한 개별 전화 통보 시 전화 통화가 3회 두절될 경우, 충원합격이 되었음에도 등록 의사가 없는 등록 포기자로 간주됩니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>동의대학교 2024학년도 정시 모집 전형에서 농어촌학생전형으로 지원할 때 제출해야 할 서류는 다음과 같습니다.
-**6년 과정 지원자의 경우:**
-1. 지원자 본인의 가족관계증명서 1부
-2. 지원자 본인, 부, 모의 주민등록초본 각 1부 (총 3부)
-3. 중학교 학교생활기록부 1부
-4. 고등학교 학교생활기록부 1부 (학생부 온라인 제공 비대상교 및 미동의자에 해당하는 경우)
-**12년 과정 지원자의 경우:**
-1. 지원자 본인의 주민등록초본 1부
-2. 초등학교 학교생활기록부 1부
-3. 중학교 학교생활기록부 1부
-4. 고등학교 학교생활기록부 1부 (학생부 온라인 제공 비대상교 및 미동의자에 해당하는 경우)【10†source】
-중·고등학교 재학 시 부모 모두 농어촌(읍·면)지역에서 거주한 자는 ‘6년과정’ 서류 제출이 가능합니다. 이 서류들은 교육기관(초·중·고교), 공공기관, 무인민원발급기, 인터넷 '정부24'에서 발급받을 수 있습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>농어촌학생전형 12년 과정으로 지원할 때는 다음의 서류들을 제출해야 합니다:
-1. 지원자 본인의 주민등록초본 1부
-2. 초등학교 학교생활기록부 1부
-3. 중학교 학교생활기록부 1부
-4. 고등학교 학교생활기록부 1부.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>검색 결과를 통해 정시 모집에서 '저소득 기회균등 전형'에 대한 구체적인 언급이 나타나지 않았습니다. 제공된 자료에는 다양한 정시 전형의 종류와 세부사항들이 나와 있지만, 저소득 기회균등 전형에 관한 정보는 확인되지 않았습니다. 더 정확한 정보를 원하신다면 2024학년도 정시 입시요강 자료를 참고하시거나 직접 동의대학교 입학관리팀에 문의하시는 것이 좋을 것 같습니다 .</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>동의대학교 2024학년도 정시 입시요강에 따르면, 등급 평균 산출 시 소수점 셋째 자리에서 절사 처리한다고 명시되어 있습니다. 따라서 사탐 2 과목의 평균을 산출할 때 2.5등급이 나오면 소수점 이하를 절사하여 2등급으로 처리한다고 이해할 수 있습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>정시 충원 합격자 발표는 1차, 2차 발표 후에 3차 이후 발표가 있습니다. 1차 등록은 2024년 2월 14일에 시작되고, 2차 발표는 2024년 2월 15일 9시에 이루어집니다. 그리고 3차 이후 충원 합격자 발표는 2024년 2월 15일 오후 7시부터 2024년 2월 20일 오후 6시까지 개별 전화 통보로 진행됩니다 .</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>e비즈니스학과의 2024학년도 정시모집에서 가장 낮은 합격 성적은 4.53입니다. 따라서 성적 4.6이면 추합 가능성이 있어 보입니다. 그러나 이 정보는 과거의 데이터에 근거한 것이므로, 실제 합격 가능성을 보장하는 것은 아닙니다. 매년 정시모집의 경쟁 상황은 달라질 수 있으니 참고만 하시고, 자세한 사항은 입학관리팀에 문의하시는 것이 좋겠습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>e비즈니스학과의 2024학년도 정시모집에서 수능 4개 영역의 등급 평균은 4.53으로 나타나고 있습니다. 따라서 5.3등급이라면, 최초합 가능성에 대해 파악하기 위해서는 과거 입시 결과보다 높은 성적이 필요할 것 같습니다. 추가적으로 정시모집 경쟁률이나 다른 변동사항을 고려해야 할 수도 있으니, 좀 더 정확한 정보를 원하시면 2024학년도 정시 입시요강을 참고하시거나 동의대학교 입학관리팀으로 문의하시는 것이 좋겠습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>동의대학교 간호학과의 2024학년도 정시 모집에서 최종 등록 인원은 145명, 경쟁률은 6.59, 최저 합격자의 성적은 481.70점이었습니다. 만약 여러분의 정시 성적이 3.44라면, 기준으로 삼은 최저 합격자 성적과의 차이가 있으므로 마지막으로 문을 닫고 들어갈 가능성은 매우 낮아 보입니다. 추가적인 질문이 있거나 더 자세한 사항을 원하신다면 동의대학교 입학관리팀에 문의해 보시는 것이 좋겠습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>정시 모집에 관한 e비즈니스학전공의 예비번호에 대한 구체적인 합격가능성을 직접 확인하는 정보는 찾을 수 없습니다. 일반적으로 예비번호의 합격가능성은 해당 대학 및 전공의 지원자 수, 합격자들의 등록 상황, 그리고 과거 연도의 예비합격자 진행 상황 등에 의해 결정되기 때문에 정확한 예측은 어렵습니다. 예비번호 38번이 예비합격 가능성이 있는지에 대해 보다 정확한 정보를 원하신다면 동의대학교 입학관리팀에 직접 문의하시는 것이 가장 좋습니다.
-만약 추가적으로 다른 질문이 있으시거나 다른 전형에 대해 알고싶으시다면 말씀해주십시오.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>간호학과의 경우 2024학년도 정시 모집에서 최종 등록자의 평균 합격 성적은 481.70점이었습니다. 성적 2.52가 어떤 점수 체계를 기준으로 한 것인지에 대한 정보가 없으므로, 합격 가능 여부를 정확히 판단하기 어렵습니다. 만약 해당 성적이 해당 학교 및 전형에서 사용하는 점수 체계와 동일하다면, 추합으로 합격하기에는 높은 점수가 필요할 것으로 보입니다. 정확한 합격 가능성을 알고자 한다면 입학관리팀에게 직접 문의하시는 것이 가장 정확할 것입니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>간호학과에 지원하기 위한 2024학년도 정시 전형의 경우, 2023년도 기준 최초 합격자의 평균 성적은 481.70점이었으며 성적 분포 상위 한계점은 6.87%로 나타났습니다. 단순히 3.7이라고 표현한 성적으로는 정확한 분석이 어려우므로, 이러한 성적 분포를 기준으로 본인의 실제 성적이 어떻게 매겨지는지 확인하신 후, 합격 가능성을 가늠해보셔야 할 것 같습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>간호학과 정시 전형에서 최종 합격한 평균 성적은 6.87로 표시되어 있습니다. 여기서 성적은 4.5점 만점에서 환산된 값으로 보이며, 2.58과 비교해보면 정시 전형 합격 가능성에 관한 구체적인 예측은 제공할 수 없으나 합격 평균 성적보다는 낮은 점수입니다. 최종 합격 가능성에 대한 보다 정확한 정보를 원하신다면, 입학관리팀에 직접 문의하시는 것이 가장 좋습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>게임공학과에 대한 2023학년도 정시 결과에 따르면 모집인원은 3명이고, 지원인원은 16명이었습니다. 기재된 경쟁률은 5.33배였고, 충원 합격한 예비번호는 3번까지였습니다. 예비번호 7번으로는 충원 합격한 정보가 보이지 않으며, 이전 연도 자료를 참고할 때 붙을 가능성에 대한 구체적인 답변을 드리기는 어렵습니다.
-추가적으로 정확한 정보를 원하신다면 2024학년도 정시 입시요강을 참고하시거나 직접 입학관리팀에 문의하시는 것을 추천드립니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>게임공학과의 경우, 2023학년도 정시모집에서 모집인원은 3명, 지원인원은 16명이었으며, 경쟁률은 5.33이었습니다. 충원 합격(후보 순위)은 3명이었습니다. 이 정보를 기반으로 할 때, 성적이 4.16 정도인 경우의 추합 가능성에 대한 정확한 예측은 제공하기 어렵습니다. 기존 자료와 정시모집 결과만으로는 세부적인 점수 분포나 올해의 모집 상황을 알 수 없기 때문입니다. 더 정확한 예측을 위해서는 입학관리팀에 문의하시거나 지난해 성적 결과를 참고해서 근사치를 확인하는 것을 권장드립니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>경영정보학과 정시 모집에서 최초합 합격자의 평균 성적은 450.78점이며, 최저 합격자는 5.90등급이었습니다. 따라서 성적 3.75등급을 가지고 계신다면 최초합으로 합격 가능성이 있어 보입니다. 다만, 매년 입시 경쟁 상황에 따라 결과는 달라질 수 있으니 참고해 주시기 바랍니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>최종 경영정보학과 정시 모집에서 성적이 4.2인 경우, 합격 가능성을 정확하게 판단하기 어렵습니다. 제공된 자료에는 경영정보학과의 2024학년도 정시 모집 성적 분포나 합격 기준 등에 대한 구체적인 정보가 없어 보입니다. 다만, 참고자료에 따르면 2024학년도 정시 모집에서 경영정보학과의 성적 상한은 434.13점, 하한은 313.13점이며, 모집 인원은 95명입니다.
-성적 4.2가 이 성적 기준에 어떻게 부합하는지 또는 전년도 입시 결과와 비교할 수 없으니, 경영정보학과의 정확한 합격 가능성에 대해 알고 싶다면 동의대학교의 입학관리팀에 문의하는 것이 좋을 것 같습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>동의대학교 2024학년도 정시 모집에서 경영정보학과 일반학생 전형의 경우 모집 인원은 9명이었고, 지원 인원은 95명이었습니다. 이에 따라 경쟁률은 10.56이었으며, 충원 합격(후보 순위)은 33명이었습니다. 그러나 여기서 제공된 내용에는 구체적인 성적 기준이나 합격 가능성에 대한 정보는 포함되어 있지 않습니다. 세부적인 성적 기준이나 합격 가능성은 본 자료로 확인할 수 없으므로, 합격 가능성에 대한 정확한 정보를 얻으려면 입학관리팀에 문의하거나 2024학년도 정시 입시요강 자료를 참조하시길 권합니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>동의대학교 바이오응용공학부의 경우, 2024학년도 정시 모집에서 수능 4개 영역 표준(변환) 점수합의 평균은 427.50이며, 국어, 수학, 탐구(2개) 표준(변환) 점수 평균은 311.13으로 나타났습니다. 영어 등급의 평균은 3.82이고, 수능 4개 영역 등급의 평균은 4.74입니다.
-성적 3.33이 어떤 표준(변환) 점수나 수능 등급에 해당하는지 명확하지 않기 때문에, 이 정보를 바탕으로 최초합 가능성을 예측하기는 어렵습니다. 일반적으로 정시 모집에서는 수능 점수가 주요한 선발 기준으로 활용되므로, 개인의 성적을 수능 표준 점수나 등급과 비교하는 것이 중요합니다.
-자세한 사항은 입학 관리 팀에 문의하시거나, 동의대학교의 입시 안내 홈페이지를 참고하시는 것이 좋습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>동의대학교 2024학년도 정시 입시 자료에 따르면, 의료보건생활대학 방사선학과의 지난해 수능 4개 영역 표준(변환)점수의 합 평균은 467.82점이었고, 수능 4개 영역 등급 평균은 3.67이었습니다. 당신이 말씀하신 수능 등급이 평균 4.4정도라면, 이 평균보다 약간 낮습니다. 그러나 실제 입학 가능 여부는 해당 연도의 경쟁 상황, 모집 인원, 그리고 다른 지원자들의 성적에 따라 달라질 수 있으므로, 직접 지원해보시는 것을 권장드립니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>방사선학과 정시 모집에 있어서의 평균적인 점수는 수능 4개 영역 표준(변환)점수 합이 평균 467.82, 국어, 수학, 탐구(2개)의 표준(변환)점수 평균이 341.62, 영어 등급 평균이 2.60 그리고 수능 4개 영역 등급 평균이 3.67 이었습니다. 2.66이라는 점수가 어떠한 기준점수인지 명확하지 않지만, 제시된 평균 점수를 기준으로 볼 때 경쟁이 높은 학과로 보여 위험할 수 있습니다. 좀 더 구체적인 정보가 필요하시다면, 2024학년도 정시 입시요강을 참조하거나 입학관리팀에 문의하시는 것을 추천 드립니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>작년과 올해의 지원 경쟁률에 대해 순수하게 비교하는 것만으로는 합격 가능성을 판단하기 어렵습니다. 경쟁률은 지원자 수와 모집 인원이 어떻게 변했는지, 그리고 지원자들의 평균 성적이 어떤지 등 여러 요인에 따라 달라질 수 있기 때문이에요.
-하지만 경쟁률이 예년에 비해 낮아졌다는 것은 해당 전형에 경쟁자가 줄었다는 것을 의미하므로, 상대적으로 선발 가능성이 증가했을 수 있다는 점에서 긍정적으로 볼 수 있습니다.
-합격 가능성에 대한 더 정확한 판단을 위해서는 자신의 성적과 지원 대학 및 학과의 전년도 입시 결과, 올해 모집 요강에 따른 평가 기준 등을 종합적으로 고려해야 합니다. 따라서 자세한 문의나 추가적인 정보가 필요하시다면 동의대학교 입학관리팀에 문의해 보는 것도 좋은 방법입니다.
-현재로서는 제가 제공드릴 수 있는 구체적인 데이터는 없으며 죄송하게도 이 문서에서는 정시 나군 학생부교과 농어촌학생전형에 대한 구체적인 경쟁률에 대한 정보를 찾을 수 없었습니다 . 현재의 경쟁률이 합격에 충분한지 여부는 다른 지원자들의 성적 분포 및 면접 등의 평가 요소에 따라 달라질 수 있음을 기억하시기 바랍니다. 여기에 더하여 본인의 지원 조건, 면접 준비 상태 등도 중요한 요소가 될 것입니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>예비 25번이신 경우, 최초 합격자를 포함하여 지원자들의 등록, 포기 또는 환불로 결원이 생긴 경우 예비후보 순위에 따라 충원합격자로 선발될 기회가 있습니다. 예비 순위가 다른 지원자들에 비해 높은지 여부, 그리고 타 합격자들의 등록 여부에 따라 변동이 있을 수 있기 때문에 정확한 확률을 예측하는 것은 어렵습니다. 충원합격자 선발 과정에서 개인 연락은 실시하지 않으니, 정시적인 일정을 확인하시고 합격 여부를 확인하시는 것이 중요합니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>정시 입시 자료 내에서 법경찰행정학부나 해당 학부의 합격 성적과 관련된 구체적인 정보를 찾지 못했습니다. 본 서비스는 정시 요강자료의 특정 내용을 찾는 데 국한되어 있어, 평균 성적이나 안정권에 대한 구체적인 수치를 제공하지 않습니다. 이에 대한 더 자세한 정보를 원하신다면, 2024학년도 정시 입시요강 자료를 참고하시거나 동의대학교 입학관리팀에 직접 문의하시는 것이 좋겠습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2023학년도 정시 모집에서 보육·가정상담학과의 합격 컷은 7.08이었습니다. 사용자님의 동의대식 정시 산출 등급이 5.33이라고 하셨는데, 이는 합격선보다 낮은 점수이므로, 이 점수만으로는 2023학년도 입시 상황에서 합격할 수 없었을 가능성이 높습니다. 그러나 2024학년도 입시의 경우, 경쟁률, 평균등급, 학생들의 성적 분포 등 여러 요인에 따라 합격선이 달라질 수 있으므로, 그 해의 입시 상황을 고려해야 합니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2023학년도 정시 모집에서 보육가정상담학과가 정원 미달을 기록했다는 내용에 따라, 예비 12번으로 3차 충원을 기다리시는 상황에서 합격 가능성은 있어 보입니다. 그러나 정확한 충원 순위나 현재 진행 상황은 제공된 자료에는 나와 있지 않아 확인이 어렵습니다. 따라서 가장 빠른 방법은 동의대학교 입학관리팀에 직접 연락하여 현재의 예비 순위와 관련하여 합격 가능성에 대해 문의하는 것입니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>성적이 4.75인 경우, 유아교육학과에 지원하기에 어려움이 있을 것 같습니다. 이전에 모집되었던 자료에 따르면 유아교육과의 수능 4개 영역 표준(변환)점수합 평균은 444.00이었습니다. 해당 점수는 보통 수능의 백분위 점수를 변환한 것으로 보입니다. 만약 사용자의 4.75라는 점수가 수능의 표준점수를 나타내는 것이라면, 평균 점수와 비교했을 때 입학이 어려울 수 있습니다. 좀 더 자세한 정보와 정확한 지원 가능성을 알고 싶다면 2024학년도 정시 입시요강을 참고하시거나 동의대학교 입학관리팀에 문의하시기 바랍니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>보육가정상담학과 일반학생전형의 경우, 2024학년도 정시 모집에서 최종 합격자의 환산등급은 6.51, 추합까지 갔을 때의 환산등급은 340.45점으로 기록되어 있고, 지원자들 간의 경쟁률은 36.36임을 확인할 수 있습니다.
-여러분의 환산등급 4.16은 제공된 자료상으로는 합격 가능성을 판단할 수 있는 직접적인 정보가 없습니다. 자세한 상담이나 추가적인 정보가 필요하시다면 동의대학교 입학관리팀에 문의하시는 것이 좋을 것 같습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2024학년도 정시 모집을 통해 동의대학교 ICT융합공과대학 소프트웨어공학부에 지원할 수 있으며, 모집인원은 총 31명입니다. 지원에 필요한 평균 등급에 대한 구체적인 내용은 제공된 자료에 명시되어 있지 않습니다. 일반적으로 대학의 정시 모집에서는 수능 최저학력 기준을 설정하여 지원자를 선발하는 경우가 있으나, 해당 전형에는 수능 최저학력 기준이 없으며, 수능 성적을 100% 반영하여 선발한다고 명시되어 있습니다 .
-정시 가군 수능 일반학생전형은 동점자 처리기준으로 다음과 같은 우선순위를 적용합니다:
-1. 수능 국어(표준점수), 수학(표준점수), 영어(등급에 따른 점수) 영역의 합계 점수 상위자
-2. ICT융합공과대학은 수능 수학(미적분 또는 기하) 응시자를 우선으로 하며,
-3. 수능 수학 영역 표준점수 상위자를 우선합니다.
-만일 동점자 처리기준 적용 시에도 최종 등수에 동점자가 발생하는 경우, 해당 인원은 모두 합격 처리됩니다.
-따라서 구체적인 등급이나 점수를 알기 위해서는 대학의 과거 입시 결과를 참조하거나, 동의대학교 입학관리팀에 직접 문의하시는 것을 추천드립니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>동의대학교 소프트웨어공학부의 정시 모집에서 2024학년도 최근 경쟁률은 4.87:1이며, 최초합격자의 평균 성적은 434.70입니다. 사용자님이 제시한 성적 4.08로 최초합격 가능성에 대해서는 정확한 예측을 제공할 수 없습니다. 각 수험생의 성적 및 정시 모집 요강에 따른 여러 인자가 최초합격 여부에 영향을 미칠 수 있기 때문에, 해당 성적만으로는 확실한 합격 여부를 판단하기 어렵습니다. 추가적인 문의가 있다면 입학관리팀에 직접 문의해 보시는 것을 권장합니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>동의대학교 2024학년도 정시 모집에서 소프트웨어공학부의 평균 등급은 4.87입니다. 평균 5등급으로 입학 가능성에 대한 정확한 예측은 제공할 수 없으나, 평균 등급이 5등급보다는 높기 때문에 경쟁이 치열할 수 있습니다. 정확한 입학 가능성을 알고 싶다면 입학관리팀에게 문의하시는 것이 좋습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>동의대학교 신소재공학과의 입시에서 영어 등급의 평균은 4.33으로 기록되어 있습니다. 따라서 성적이 4.28이신 경우, 영어 등급이 평균보다 약간 높은 점수임을 알 수 있으나, 합격 가능성을 평가하기 위해서는 다른 과목의 성적, 수능 전체 평균 등급 및 수능 표준 점수 등 전체적인 성적을 고려해야 합니다. 이 정보만으로는 정확한 합격 가능성을 예측하기 어렵습니다.
-추가적으로, 통상적으로 입시에서는 성적뿐만 아니라 모집 단위별 경쟁률과 올해의 지원 추세 등 다양한 요소가 합격 기준에 영향을 미칩니다. 정확한 합격 가능성을 알고 싶으시다면, 필요한 모든 성적 정보를 갖추고 입학관리팀에 문의하시거나, 과거 입시 결과와 비교해 볼 것을 권장합니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>정시 다군 수능 일반학생 전형은 별도의 제출서류가 없으며, 이는 자기소개서를 포함하지 않습니다 . 따라서 수능 일반학생전형으로 지원할 때 자기소개서를 작성할 필요가 없습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>추가모집 가능성에 대해서는 정시 모집인원이 수시모집 등록 결과에 따라 증가할 수 있음을 밝히고 있습니다. 구체적인 정시 추가모집 인원은 2024년 1월 2일 화요일에 동의대학교 입학 안내 홈페이지를 통해 공고될 예정입니다. 따라서, 수능 산출 점수 4.5를 가지고 추가모집에서 지원 가능성을 알아보시려면 해당 일자에 홈페이지를 확인하시거나 직접 입학관리팀에 문의하시는 것이 좋을 것 같습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>동의대학교 신소재공학부의 정시모집에서 신소재공학과의 지난해 경쟁률은 1.45:1 이었고, 모집인원은 56명, 지원인원은 81명이었습니다. 합격자 평균등급은 16.29였습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>작년 동의대학교 신소재공학과의 평균 정시 표준점수는 399.26점이었습니다. 사용자님의 표준점수가 447점으로, 이는 작년의 평균 정시 표준점수보다 높으므로, 올해 입시에서 신소재공학과에 합격할 가능성은 있어 보입니다. 하지만, 매년 입시 경쟁률과 지원자들의 평균 성적은 바뀔 수 있으므로, 최종 합격 가능성에 대해서는 보장할 수 없음을 양해해 주시기 바랍니다. 추가적으로 입시 결과는 다양한 요소에 의해 결정되며, 최신 입시 동향과 경쟁률을 반드시 확인하세요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>동의대학교 공과대학 신소재공학부의 지난 정시모집에서 수능 4개 영역 표준(변환)점수합의 평균은 399.26, 국어, 수학, 탐구(2개) 표준(변환)점수 평균은 286.97, 영어 등급 평균은 4.33, 수능 4개 영역 등급 평균은 5.32였습니다. 여러분의 현재 성적 예상이 정확히 맞는다고 해도, 이전의 평균적인 합격 성적과 비교했을 때 경쟁이 있을 것으로 보입니다. 따라서 단순한 비교만으로 합격 가능성을 정확히 판단하기는 어렵습니다. 매년 입시 경쟁률과 학생들의 수능 성적 분포가 변할 수 있기 때문에, 이는 단지 참고 사항일 뿐 실제 합격 가능성과는 다를 수 있음을 유념하시기 바랍니다.
-추가적으로, 여러분의 최종 합격 가능성은 다른 지원자들의 성적과 동의대학교의 선발 기준에 따라 달라질 수 있으며, 보다 정확한 정보를 원하시면 입학관리팀에 문의하시는 것이 좋을 것 같습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>동의대학교 인공지능학과 정시 가군 수능 일반학생 전형은 수능 점수를 100% 반영하며, 수능 최저학력기준은 없습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>동의대학교 창의소프트웨어공학부의 2024학년도 정시모집에서는 모집인원이 30명이고, 경쟁률은 4.87:1로 나타났습니다. 또한, 그 해 최초 합격자의 평균 교과 성적은 7.35, 최고 교과 성적은 3.77, 최저 교과 성적은 0.67의 수치를 보였습니다.
-교과 성적이 4.2인 경우에도 여러 요소가 복합적으로 고려되기 때문에 정확한 합격 가능성을 단정적으로 말하기 어렵지만, 최저 교과 성적이 0.67로 나타나는 것을 고려하면 전형에 따라 가능성이 있을 수 있습니다. 다만 정시 모집에서는 수능 성적이 중요한 요인으로 작용할 수 있으므로, 추가적인 정보를 참고하셔야 할 것입니다. 정확한 입시 상담을 위해서는 입학관리팀에 문의하시는 것이 좋습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>추가 합격(추합) 여부는 본인이 직접 동의대학교 홈페이지에서 확인해야 합니다. 정시 충원 합격자 발표는 다음과 같은 일정으로 진행됩니다:
-- 1차 충원 합격자 발표: 2024년 2월 14일 오전 9시
-- 2차 충원 합격자 발표: 2024년 2월 15일 오전 9시
-- 3차 이후 충원 합격자 발표: 2024년 2월 15일 오후 7시 부터 2월 20일 오후 6시까지 개별 전화 통보
-합격자 발표는 동의대학교 입학 홈페이지에서 개별 조회 가능하며, 최초 합격자와 1차, 2차 충원 합격자에게는 별도로 연락을 하지 않으므로 지원자는 지정된 발표일에 합격 여부를 확인해야 합니다.
-사용자의 점수 5.27이 추합 가능성에 대해서는 이 자료에서 구체적인 기준이나 점수대를 제시하고 있지 않으므로, 동의대학교 입학관리팀에 문의하거나 지정된 합격자 발표일에 홈페이지에서 직접 확인해보시는 것을 권장합니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>동의대학교 공과대학 화학환경공학부의 2023학년도 정시 모집에서 수능 일반학생전형 최종등록자의 수능 4개 영역 등급 평균은 5.59였습니다. 따라서 귀하의 수능 성적이 4.25인 경우, 이전 년도 기준으로 볼 때 경쟁력이 있을 것으로 보입니다. 그러나 이는 단순 참고용으로, 실제 입학 가능 여부는 해당 학년도의 지원자 수준과 모집인원에 따라 달라질 수 있으니 이 점 유념하시기 바랍니다. 정확한 정보를 원하시면 입학관리팀에 문의하시는 것이 좋습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>동의대학교 공과대학 화학환경공학부의 2023학년도 정시 입시에서 일반학생전형의 수능 4개 영역 표준(변환)점수합 평균은 385.99이고, 국어+수학+탐구(2개) 표준(변환)점수 평균은 276.61, 영어등급 평균은 4.70, 수능 4개 영역 등급 평균은 5.59였습니다. 여러분의 성적 3.92는 이 평균보다 높으므로, 화학환경공학부 일반학생전형에 지원할 가능성이 있어 보입니다. 하지만 최종적인 합격 여부는 수험생의 경쟁 상황이나 해당 연도의 모집 정원, 그리고 다른 지원자의 성적 분포 등 다양한 요소에 따라 달라질 수 있으니, 정확한 합격 가능성을 알고 싶다면 입학관리팀에 문의하시기 바랍니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>영화학과 정시 지원에서 수능 4개 영역 등급 평균이 4.47이었습니다. 사용자께서 말씀하신 성적 4.2는 이 평균보다 조금 낮으므로 경쟁력이 있다고 볼 수 있습니다. 그렇지만 최종적인 합격 가능성은 다양한 요소들, 예를 들어 지원자 수, 해당 연도의 경쟁률, 그리고 여러분의 전체적인 성적 분포에 따라 결정될 것 입니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>면접 절차는 다음과 같습니다:
-1. 대기실 입실
-2. 신분 확인
-3. 고사장 앞 이동
-4. 고사장 입실
-5. 지원동기 및 학업계획 발표
-6. 학업역량, 전공적합성 관련 공통문항 발표 및 질의응답
-7. 기타 질의응답(제출서류 진위 여부 등)
-8. 퇴실 .
-과정 중에서 면접은 면접위원 2~3인이 평가위원이 되어 수험생 1명을 대상으로 개별적으로 평가하며, 수험생의 답변 내용을 바탕으로 정성적이고 종합적으로 평가합니다. 또한 지원자별로 채용기업 심층면접이 이루어질 수 있으며, 이 과정에서도 면접위원 2~3인이 참여합니다 .
-추가적으로, 면접 시에는 개인신상정보에 대한 노출을 금지하며, 교복 착용도 금지됩니다 .</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -2106,7 +1430,7 @@
 12. 창의소프트웨어공학부(컴퓨터소프트웨어공학, 응용소프트웨어공학) → 소프트웨어공학부(컴퓨터소프트웨어공학, 응용소프트웨어공학)
 13. 전기전자통신공학부(전기공학, 전자공학, 정보통신공학) → 전기공학과, 전자공학과
 14. 음악학과(성악, 피아노, 관현타악, 실용음악뮤지컬, 뉴미디어작곡) → 음악학과(클래식, 실용음악, 뉴미디어작곡)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>동의대학교는 수능 최저기준이 없습니다.</t>
@@ -2114,7 +1438,7 @@
   </si>
   <si>
     <t>동의대학교 2024학년도 나군 수능(일반학생전형) 전형에서는 한의예과, 디자인조형학과와 체육학과, 경기지도학과가 제외됩니다.</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">동의대 2024학년도에 전형 요소 변화가 있는 전형은 다음과 같습니다:
@@ -2152,7 +1476,7 @@
    -국어, 수학, 영어, 한국사, 사회(역사/도덕 포함), 과학, 한문교과 전과목
    -진로선택과목: 반영교과 전과목 반영
 </t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>동의대 2024학년도 가군에서 실기고사에 참여해야 하는 학과는 다음과 같습니다:
@@ -2187,7 +1511,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2202,19 +1526,6 @@
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF212529"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF212529"/>
-      <name val="맑은 고딕"/>
-      <family val="2"/>
-      <charset val="129"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2259,24 +1570,21 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2595,8 +1903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6B1BFF4-AFEB-47CA-A3A5-20AA54A6AED6}">
   <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2722,7 +2030,7 @@
         <v>28</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>318</v>
+        <v>222</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -2730,7 +2038,7 @@
         <v>30</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>320</v>
+        <v>224</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="132">
@@ -2777,8 +2085,8 @@
       <c r="A22" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>321</v>
+      <c r="B22" s="3" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="66">
@@ -2793,8 +2101,8 @@
       <c r="A24" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>319</v>
+      <c r="B24" s="3" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="33">
@@ -2809,8 +2117,8 @@
       <c r="A26" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>322</v>
+      <c r="B26" s="4" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="33">
@@ -2834,15 +2142,15 @@
         <v>56</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>323</v>
+        <v>227</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="132">
       <c r="A30" t="s">
         <v>58</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>324</v>
+      <c r="B30" s="4" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="82.5">
@@ -2913,16 +2221,16 @@
       <c r="A39" t="s">
         <v>76</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>325</v>
+      <c r="B39" s="2" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
         <v>78</v>
       </c>
-      <c r="B40" s="3" t="s">
-        <v>325</v>
+      <c r="B40" s="2" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="132">
@@ -2951,7 +2259,7 @@
     </row>
     <row r="44" spans="1:2" ht="409.5">
       <c r="A44" t="s">
-        <v>297</v>
+        <v>201</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>87</v>
@@ -2959,7 +2267,7 @@
     </row>
     <row r="45" spans="1:2" ht="99">
       <c r="A45" t="s">
-        <v>298</v>
+        <v>202</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>89</v>
@@ -2967,7 +2275,7 @@
     </row>
     <row r="46" spans="1:2" ht="33">
       <c r="A46" t="s">
-        <v>299</v>
+        <v>203</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>91</v>
@@ -2975,7 +2283,7 @@
     </row>
     <row r="47" spans="1:2" ht="33">
       <c r="A47" t="s">
-        <v>300</v>
+        <v>204</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>91</v>
@@ -2991,7 +2299,7 @@
     </row>
     <row r="49" spans="1:2" ht="49.5">
       <c r="A49" t="s">
-        <v>301</v>
+        <v>205</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>96</v>
@@ -3015,7 +2323,7 @@
     </row>
     <row r="52" spans="1:2" ht="409.5">
       <c r="A52" t="s">
-        <v>302</v>
+        <v>206</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>102</v>
@@ -3023,7 +2331,7 @@
     </row>
     <row r="53" spans="1:2" ht="409.5">
       <c r="A53" t="s">
-        <v>303</v>
+        <v>207</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>104</v>
@@ -3039,10 +2347,10 @@
     </row>
     <row r="55" spans="1:2" ht="82.5">
       <c r="A55" t="s">
-        <v>327</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>326</v>
+        <v>231</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="66">
@@ -3063,7 +2371,7 @@
     </row>
     <row r="58" spans="1:2" ht="409.5">
       <c r="A58" t="s">
-        <v>317</v>
+        <v>221</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>114</v>
@@ -3071,7 +2379,7 @@
     </row>
     <row r="59" spans="1:2" ht="247.5">
       <c r="A59" t="s">
-        <v>304</v>
+        <v>208</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>116</v>
@@ -3103,7 +2411,7 @@
     </row>
     <row r="63" spans="1:2" ht="409.5">
       <c r="A63" t="s">
-        <v>316</v>
+        <v>220</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>124</v>
@@ -3111,7 +2419,7 @@
     </row>
     <row r="64" spans="1:2" ht="148.5">
       <c r="A64" t="s">
-        <v>307</v>
+        <v>211</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>126</v>
@@ -3119,7 +2427,7 @@
     </row>
     <row r="65" spans="1:2" ht="99">
       <c r="A65" t="s">
-        <v>305</v>
+        <v>209</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>128</v>
@@ -3127,7 +2435,7 @@
     </row>
     <row r="66" spans="1:2" ht="148.5">
       <c r="A66" t="s">
-        <v>306</v>
+        <v>210</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>130</v>
@@ -3135,7 +2443,7 @@
     </row>
     <row r="67" spans="1:2" ht="148.5">
       <c r="A67" t="s">
-        <v>308</v>
+        <v>212</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>131</v>
@@ -3143,15 +2451,15 @@
     </row>
     <row r="68" spans="1:2" ht="132">
       <c r="A68" t="s">
-        <v>296</v>
+        <v>200</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="132">
       <c r="A69" t="s">
-        <v>309</v>
+        <v>213</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>133</v>
@@ -3175,7 +2483,7 @@
     </row>
     <row r="72" spans="1:2" ht="148.5">
       <c r="A72" t="s">
-        <v>310</v>
+        <v>214</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>139</v>
@@ -3263,7 +2571,7 @@
     </row>
     <row r="83" spans="1:2" ht="409.5">
       <c r="A83" t="s">
-        <v>311</v>
+        <v>215</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>161</v>
@@ -3271,7 +2579,7 @@
     </row>
     <row r="84" spans="1:2" ht="165">
       <c r="A84" t="s">
-        <v>312</v>
+        <v>216</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>163</v>
@@ -3327,7 +2635,7 @@
     </row>
     <row r="91" spans="1:2" ht="297">
       <c r="A91" t="s">
-        <v>313</v>
+        <v>217</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>177</v>
@@ -3335,7 +2643,7 @@
     </row>
     <row r="92" spans="1:2" ht="132">
       <c r="A92" t="s">
-        <v>314</v>
+        <v>218</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>179</v>
@@ -3343,7 +2651,7 @@
     </row>
     <row r="93" spans="1:2" ht="115.5">
       <c r="A93" t="s">
-        <v>315</v>
+        <v>219</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>181</v>
@@ -3428,10 +2736,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FA047E5-64A6-46F6-B6F2-6A9E7AD22C76}">
-  <dimension ref="A1:B100"/>
+  <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="A101" sqref="A101"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B101" sqref="A1:B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -3439,804 +2747,812 @@
     <col min="1" max="1" width="103.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="409.5">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="409.5">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="49.5">
-      <c r="A2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="409.5">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="49.5">
-      <c r="A3" t="s">
+      <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="409.5">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="181.5">
-      <c r="A4" t="s">
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="409.5">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="346.5">
-      <c r="A5" t="s">
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="115.5">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="181.5">
-      <c r="A6" t="s">
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="148.5">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="198">
-      <c r="A7" t="s">
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="181.5">
+      <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
+      <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="181.5">
+      <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="409.5">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
       <c r="B9" s="1" t="s">
-        <v>207</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="409.5">
       <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="409.5">
+      <c r="A11" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="49.5">
-      <c r="A11" t="s">
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="231">
+      <c r="A12" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="181.5">
-      <c r="A12" t="s">
+      <c r="B12" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="99">
+      <c r="A13" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="132">
-      <c r="A13" t="s">
+      <c r="B13" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="132">
+      <c r="A14" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="214.5">
-      <c r="A14" t="s">
+      <c r="B14" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="264">
+      <c r="A15" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="165">
-      <c r="A15" t="s">
+      <c r="B15" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="82.5">
+      <c r="A16" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="409.5">
-      <c r="A16" t="s">
+      <c r="B16" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="409.5">
+      <c r="A17" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="115.5">
-      <c r="A17" t="s">
+      <c r="B17" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="198">
+      <c r="A18" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="396">
-      <c r="A18" t="s">
-        <v>36</v>
-      </c>
       <c r="B18" s="1" t="s">
-        <v>215</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="409.5">
       <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="330">
+      <c r="A20" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="231">
-      <c r="A20" t="s">
+      <c r="B20" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="132">
+      <c r="A21" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="396">
-      <c r="A21" t="s">
+      <c r="B21" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="231">
+      <c r="A22" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="148.5">
-      <c r="A22" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>219</v>
+      <c r="B22" s="3" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="409.5">
       <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="409.5">
+      <c r="A24" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="165">
-      <c r="A24" t="s">
+      <c r="B24" s="3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="165">
+      <c r="A25" t="s">
         <v>48</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="409.5">
-      <c r="A25" t="s">
+      <c r="B25" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="409.5">
+      <c r="A26" t="s">
         <v>50</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="214.5">
-      <c r="A26" t="s">
+      <c r="B26" s="4" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="132">
+      <c r="A27" t="s">
         <v>52</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="264">
-      <c r="A27" t="s">
+      <c r="B27" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="297">
+      <c r="A28" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="346.5">
-      <c r="A28" t="s">
+      <c r="B28" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="231">
+      <c r="A29" t="s">
         <v>56</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="409.5">
-      <c r="A29" t="s">
+      <c r="B29" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="330">
+      <c r="A30" t="s">
         <v>58</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="409.5">
-      <c r="A30" t="s">
+      <c r="B30" s="4" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="280.5">
+      <c r="A31" t="s">
         <v>60</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="409.5">
-      <c r="A31" t="s">
+      <c r="B31" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="409.5">
+      <c r="A32" t="s">
         <v>62</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="231">
-      <c r="A32" t="s">
+      <c r="B32" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="297">
+      <c r="A33" t="s">
         <v>64</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="409.5">
-      <c r="A33" t="s">
-        <v>66</v>
-      </c>
       <c r="B33" s="1" t="s">
-        <v>230</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="409.5">
       <c r="A34" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>231</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="409.5">
       <c r="A35" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="409.5">
+      <c r="A36" t="s">
         <v>70</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="165">
-      <c r="A36" t="s">
+      <c r="B36" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="409.5">
+      <c r="A37" t="s">
         <v>72</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="297">
-      <c r="A37" t="s">
+      <c r="B37" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="297">
+      <c r="A38" t="s">
         <v>74</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="330">
-      <c r="A38" t="s">
+      <c r="B38" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
         <v>76</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="132">
-      <c r="A39" t="s">
+      <c r="B39" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
         <v>78</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="280.5">
-      <c r="A40" t="s">
-        <v>80</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>237</v>
+      <c r="B40" s="2" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="409.5">
       <c r="A41" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>238</v>
+        <v>81</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="409.5">
       <c r="A42" t="s">
+        <v>82</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="198">
+      <c r="A43" t="s">
         <v>84</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="165">
-      <c r="A43" t="s">
-        <v>86</v>
-      </c>
       <c r="B43" s="1" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="181.5">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="409.5">
       <c r="A44" t="s">
-        <v>88</v>
+        <v>201</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="409.5">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="379.5">
       <c r="A45" t="s">
-        <v>90</v>
+        <v>202</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="363">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="165">
       <c r="A46" t="s">
-        <v>92</v>
+        <v>203</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="115.5">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="165">
       <c r="A47" t="s">
+        <v>204</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="409.5">
+      <c r="A48" t="s">
         <v>93</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="115.5">
-      <c r="A48" t="s">
-        <v>95</v>
-      </c>
       <c r="B48" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="409.5">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="346.5">
       <c r="A49" t="s">
+        <v>205</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="231">
+      <c r="A50" t="s">
         <v>97</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="409.5">
-      <c r="A50" t="s">
-        <v>99</v>
-      </c>
       <c r="B50" s="1" t="s">
-        <v>245</v>
+        <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="409.5">
       <c r="A51" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>246</v>
+        <v>100</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="409.5">
       <c r="A52" t="s">
-        <v>103</v>
+        <v>206</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>249</v>
+        <v>102</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="409.5">
       <c r="A53" t="s">
+        <v>207</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="409.5">
+      <c r="A54" t="s">
         <v>105</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="363">
-      <c r="A54" t="s">
-        <v>107</v>
-      </c>
       <c r="B54" s="1" t="s">
-        <v>248</v>
+        <v>106</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="409.5">
       <c r="A55" t="s">
+        <v>231</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="280.5">
+      <c r="A56" t="s">
         <v>109</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="264">
-      <c r="A56" t="s">
-        <v>111</v>
-      </c>
       <c r="B56" s="1" t="s">
-        <v>251</v>
+        <v>110</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="409.5">
       <c r="A57" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>252</v>
+        <v>112</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="409.5">
       <c r="A58" t="s">
-        <v>115</v>
+        <v>221</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>253</v>
+        <v>114</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="409.5">
       <c r="A59" t="s">
+        <v>208</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="297">
+      <c r="A60" t="s">
         <v>117</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="409.5">
-      <c r="A60" t="s">
-        <v>119</v>
-      </c>
       <c r="B60" s="1" t="s">
-        <v>255</v>
+        <v>118</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="409.5">
       <c r="A61" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>256</v>
+        <v>120</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="409.5">
       <c r="A62" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>257</v>
+        <v>122</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="409.5">
       <c r="A63" t="s">
-        <v>125</v>
+        <v>220</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>258</v>
+        <v>124</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="409.5">
       <c r="A64" t="s">
-        <v>127</v>
+        <v>211</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>260</v>
+        <v>126</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="409.5">
       <c r="A65" t="s">
-        <v>129</v>
+        <v>209</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>259</v>
+        <v>128</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="409.5">
       <c r="A66" t="s">
-        <v>295</v>
+        <v>210</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>261</v>
+        <v>130</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="409.5">
       <c r="A67" t="s">
-        <v>198</v>
+        <v>212</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>262</v>
+        <v>131</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="409.5">
       <c r="A68" t="s">
-        <v>132</v>
+        <v>200</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>263</v>
+        <v>198</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="409.5">
       <c r="A69" t="s">
-        <v>134</v>
+        <v>213</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>264</v>
+        <v>133</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="409.5">
       <c r="A70" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>265</v>
+        <v>135</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="409.5">
       <c r="A71" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>266</v>
+        <v>137</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="409.5">
       <c r="A72" t="s">
-        <v>140</v>
+        <v>214</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>267</v>
+        <v>139</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="409.5">
       <c r="A73" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>268</v>
+        <v>141</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="409.5">
       <c r="A74" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>269</v>
+        <v>143</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="409.5">
       <c r="A75" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>270</v>
+        <v>145</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="409.5">
       <c r="A76" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>271</v>
+        <v>147</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="409.5">
       <c r="A77" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>272</v>
+        <v>149</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="409.5">
       <c r="A78" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>273</v>
+        <v>151</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="409.5">
       <c r="A79" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>274</v>
+        <v>153</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="409.5">
       <c r="A80" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>275</v>
+        <v>155</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="409.5">
       <c r="A81" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>276</v>
+        <v>157</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="409.5">
       <c r="A82" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>277</v>
+        <v>159</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="409.5">
       <c r="A83" t="s">
-        <v>162</v>
+        <v>215</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>278</v>
+        <v>161</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="409.5">
       <c r="A84" t="s">
-        <v>164</v>
+        <v>216</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>279</v>
+        <v>163</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="115.5">
       <c r="A85" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>214</v>
+        <v>165</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="409.5">
       <c r="A86" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>280</v>
+        <v>167</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="409.5">
       <c r="A87" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>281</v>
+        <v>169</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="409.5">
       <c r="A88" t="s">
+        <v>170</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="409.5">
+      <c r="A89" t="s">
         <v>172</v>
       </c>
-      <c r="B88" s="1" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" ht="313.5">
-      <c r="A89" t="s">
+      <c r="B89" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="115.5">
+      <c r="A90" t="s">
         <v>174</v>
       </c>
-      <c r="B89" s="1" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" ht="409.5">
-      <c r="A90" t="s">
-        <v>176</v>
-      </c>
       <c r="B90" s="1" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" ht="313.5">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="409.5">
       <c r="A91" t="s">
-        <v>178</v>
+        <v>217</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>285</v>
+        <v>177</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="409.5">
       <c r="A92" t="s">
-        <v>180</v>
+        <v>218</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>286</v>
+        <v>179</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="409.5">
       <c r="A93" t="s">
+        <v>219</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="409.5">
+      <c r="A94" t="s">
         <v>182</v>
       </c>
-      <c r="B93" s="1" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" ht="231">
-      <c r="A94" t="s">
-        <v>184</v>
-      </c>
       <c r="B94" s="1" t="s">
-        <v>288</v>
+        <v>183</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="409.5">
       <c r="A95" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>290</v>
+        <v>185</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="409.5">
       <c r="A96" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>289</v>
+        <v>187</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="409.5">
       <c r="A97" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>292</v>
+        <v>189</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="409.5">
       <c r="A98" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>291</v>
+        <v>191</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="409.5">
       <c r="A99" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>293</v>
+        <v>193</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="409.5">
       <c r="A100" t="s">
+        <v>194</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="409.5">
+      <c r="A101" t="s">
         <v>196</v>
       </c>
-      <c r="B100" s="1" t="s">
-        <v>294</v>
+      <c r="B101" s="1" t="s">
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -4251,7 +3567,7 @@
   <dimension ref="A1:B101"/>
   <sheetViews>
     <sheetView topLeftCell="A101" workbookViewId="0">
-      <selection sqref="A1:B101"/>
+      <selection activeCell="C101" sqref="C101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -4786,7 +4102,7 @@
     </row>
     <row r="67" spans="1:2" ht="409.5">
       <c r="A67" t="s">
-        <v>295</v>
+        <v>199</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>131</v>
@@ -4794,10 +4110,10 @@
     </row>
     <row r="68" spans="1:2" ht="409.5">
       <c r="A68" t="s">
-        <v>296</v>
+        <v>200</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="409.5">

</xml_diff>